<commit_message>
add excel file server details
</commit_message>
<xml_diff>
--- a/docs/testing.xlsx
+++ b/docs/testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="516" windowWidth="23256" windowHeight="11952" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="510" windowWidth="23250" windowHeight="11955" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,14 @@
     <sheet name="Info" sheetId="7" r:id="rId7"/>
     <sheet name="After Testing Success" sheetId="9" r:id="rId8"/>
     <sheet name="Primary" sheetId="10" r:id="rId9"/>
-    <sheet name="Temporary " sheetId="11" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
+    <sheet name="Server" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="182">
   <si>
     <t>Items</t>
   </si>
@@ -560,70 +559,16 @@
     <t>support@rees52.com</t>
   </si>
   <si>
-    <t>SV TESTING</t>
-  </si>
-  <si>
-    <t>SV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SV </t>
-  </si>
-  <si>
-    <t>Sno</t>
-  </si>
-  <si>
-    <t>Solenoid valve</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/divinext-1pc-230v-ac-electric-solenoid-valve-1-2-20mm-n-c-male-thread-type-normally-closed-plastic-water-air-inlet-flow-switch-off-agro-drip-irrigation-automation-gardening-ro-purifiers-electromechanically-two-port-sv-automatic-control-valves/p/itmfchmxzhzrzwg3?pid=HWVFCHANRQU5X7Z8&amp;lid=LSTHWVFCHANRQU5X7Z8UL7GUT&amp;marketplace=FLIPKART&amp;q=Divinext+12V+DC+SV+Valve+1%2F2x1%2F2+Electric+Solenoid+Valve+Normally+Closed+12+Volt+DC+Water+Automatic+Control+Valves&amp;store=b8s%2Fzp2%2Fhlx&amp;srno=s_1_3&amp;otracker=search&amp;otracker1=search&amp;fm=productRecommendation%2Fsimilar&amp;iid=b169a058-45ba-4f8b-8a0d-da0b4737d5b1.HWVFCHANRQU5X7Z8.SEARCH&amp;ppt=pp&amp;ppn=pp&amp;ssid=xrgvwj9bnv0qgsu81732855070481&amp;qH=ab0904320e19bf53</t>
-  </si>
-  <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Prouct</t>
-  </si>
-  <si>
-    <t>qty</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>net price</t>
-  </si>
-  <si>
-    <t>dealer</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>robu</t>
-  </si>
-  <si>
-    <t>https://robu.in/product/dfrobot-fermion-microsd-card-module-for-arduino-breakout/</t>
-  </si>
-  <si>
-    <t>MicroSD Breakout Board-serverside</t>
-  </si>
-  <si>
-    <t>Ethernet Connector</t>
-  </si>
-  <si>
-    <t>https://robu.in/product/ethernet-module-enc28j60/</t>
-  </si>
-  <si>
-    <t>WiFi Booster</t>
-  </si>
-  <si>
-    <t>Raspberri Pi Zero 2 W</t>
-  </si>
-  <si>
-    <t>robocraze</t>
-  </si>
-  <si>
-    <t>https://robocraze.com/products/raspberry-pi-zero-2-w?src=raspberrypi</t>
+    <t>SERVER</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3 A +</t>
   </si>
 </sst>
 </file>
@@ -951,8 +896,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="48"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1036,7 +982,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,14 +1100,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="9" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="1" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Accent1" xfId="8" builtinId="29"/>
@@ -1384,17 +1323,17 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.09765625" customWidth="1"/>
-    <col min="2" max="2" width="8.69921875" customWidth="1"/>
-    <col min="3" max="3" width="180.09765625" customWidth="1"/>
+    <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="180.125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="8.69921875" customWidth="1"/>
-    <col min="7" max="26" width="14.3984375" customWidth="1"/>
+    <col min="5" max="6" width="8.75" customWidth="1"/>
+    <col min="7" max="26" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.8">
+    <row r="1" spans="1:5" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,10 +1350,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1371,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1385,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1399,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1413,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.4">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1488,7 +1427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.4">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1502,7 +1441,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1516,7 +1455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.4">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1544,7 +1483,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.4">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1558,7 +1497,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.4">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1618,7 +1557,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.4">
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1632,7 +1571,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.4">
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2795,41 +2734,44 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD78"/>
+  <sheetPr>
+    <tabColor theme="2" tint="-0.14999847407452621"/>
+  </sheetPr>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="76.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="20.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="19" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
+    <col min="6" max="6" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="54.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20 16384:16384" ht="91.2" thickTop="1" thickBot="1">
-      <c r="A1" s="84" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="84" t="s">
+    <row r="1" spans="1:15" ht="61.5" thickTop="1" thickBot="1">
+      <c r="A1" s="97" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="97" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" s="84" t="s">
-        <v>179</v>
+      <c r="C1" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="97" t="s">
+        <v>178</v>
       </c>
       <c r="H1" s="97" t="s">
         <v>178</v>
@@ -2855,207 +2797,71 @@
       <c r="O1" s="97" t="s">
         <v>178</v>
       </c>
-      <c r="P1" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q1" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="R1" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="S1" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="T1" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="XFD1" s="91" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20 16384:16384" ht="14.4" thickTop="1"/>
-    <row r="4" spans="1:20 16384:16384">
-      <c r="A4" s="71" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="15" thickTop="1"/>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="71" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20 16384:16384" ht="138.6">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20 16384:16384" ht="14.4">
-      <c r="B6" s="100"/>
-    </row>
-    <row r="78" spans="3:3">
-      <c r="C78" s="98" t="s">
-        <v>183</v>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="12" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col min="1" max="1" width="39.19921875" customWidth="1"/>
-    <col min="2" max="2" width="30.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="90">
-      <c r="A1" s="101" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>400</v>
-      </c>
-      <c r="E4">
-        <f>C4*D4</f>
-        <v>400</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>330</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E7" si="0">C5*D5</f>
-        <v>330</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1600</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="F7" s="91" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="102" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3067,18 +2873,18 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.09765625" customWidth="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1"/>
-    <col min="3" max="3" width="180.09765625" customWidth="1"/>
+    <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="180.125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18.8984375" customWidth="1"/>
-    <col min="6" max="6" width="8.69921875" customWidth="1"/>
-    <col min="7" max="26" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="7" max="26" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.8">
+    <row r="1" spans="1:5" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3095,7 +2901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -3112,7 +2918,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -3130,7 +2936,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -3148,7 +2954,7 @@
         <v>19170</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3166,7 +2972,7 @@
         <v>7560</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -3184,7 +2990,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.4">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -3202,7 +3008,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.4">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -3220,7 +3026,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3238,7 +3044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4408,18 +4214,18 @@
       <selection activeCell="A10" sqref="A10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.09765625" customWidth="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1"/>
-    <col min="3" max="3" width="26.19921875" customWidth="1"/>
+    <col min="1" max="1" width="34.125" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="26.25" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18.8984375" customWidth="1"/>
-    <col min="6" max="6" width="8.69921875" customWidth="1"/>
-    <col min="7" max="26" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="7" max="26" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.8">
+    <row r="1" spans="1:5" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4436,7 +4242,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -4454,7 +4260,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -4472,7 +4278,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -5607,23 +5413,23 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="14.69921875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="22.09765625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="14.75" style="26" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.125" style="14" customWidth="1"/>
     <col min="6" max="6" width="37.5" style="14" customWidth="1"/>
     <col min="7" max="7" width="24.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.69921875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="38.69921875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="14" customWidth="1"/>
+    <col min="9" max="9" width="38.75" style="14" customWidth="1"/>
     <col min="10" max="10" width="40" style="14" customWidth="1"/>
-    <col min="11" max="11" width="38.8984375" style="14" customWidth="1"/>
-    <col min="12" max="12" width="38.69921875" style="23" customWidth="1"/>
-    <col min="13" max="14" width="38.69921875" style="14" customWidth="1"/>
-    <col min="15" max="28" width="14.3984375" style="14" customWidth="1"/>
-    <col min="29" max="16384" width="12.59765625" style="14"/>
+    <col min="11" max="11" width="38.875" style="14" customWidth="1"/>
+    <col min="12" max="12" width="38.75" style="23" customWidth="1"/>
+    <col min="13" max="14" width="38.75" style="14" customWidth="1"/>
+    <col min="15" max="28" width="14.375" style="14" customWidth="1"/>
+    <col min="29" max="16384" width="12.625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
@@ -5680,7 +5486,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.4">
+    <row r="4" spans="1:14">
       <c r="A4" s="80" t="s">
         <v>51</v>
       </c>
@@ -5811,7 +5617,7 @@
       <c r="F12" s="42"/>
       <c r="L12" s="44"/>
     </row>
-    <row r="13" spans="1:14" ht="14.4">
+    <row r="13" spans="1:14">
       <c r="A13" s="15" t="s">
         <v>68</v>
       </c>
@@ -5830,7 +5636,7 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:14" s="43" customFormat="1" thickBot="1">
+    <row r="14" spans="1:14" s="43" customFormat="1" ht="15.75" thickBot="1">
       <c r="A14" s="45"/>
       <c r="B14" s="46"/>
       <c r="C14" s="47"/>
@@ -6960,13 +6766,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="34"/>
-    <col min="3" max="3" width="10.3984375" style="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7018,7 +6824,7 @@
       </c>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
+    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>57</v>
       </c>
@@ -7036,7 +6842,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
+    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -7054,7 +6860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
+    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
@@ -7072,7 +6878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
+    <row r="10" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
@@ -7090,7 +6896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" thickTop="1">
+    <row r="11" spans="1:12" ht="15.75" thickTop="1">
       <c r="A11" s="13" t="s">
         <v>42</v>
       </c>
@@ -7123,7 +6929,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18">
+    <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="52" t="s">
         <v>99</v>
       </c>
@@ -7149,16 +6955,16 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.4">
+    <row r="1" spans="1:12" ht="35.25">
       <c r="A1" s="66" t="s">
         <v>103</v>
       </c>
@@ -7193,7 +6999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:12" ht="18.75">
       <c r="A2" s="67" t="s">
         <v>105</v>
       </c>
@@ -7219,7 +7025,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="68">
         <v>45587</v>
       </c>
@@ -7245,7 +7051,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="68">
         <v>45587</v>
       </c>
@@ -7271,7 +7077,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="70.2">
+    <row r="5" spans="1:12" ht="87">
       <c r="A5" s="68">
         <v>45587</v>
       </c>
@@ -7297,7 +7103,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="42.6">
+    <row r="6" spans="1:12" ht="58.5">
       <c r="A6" s="68">
         <v>45588</v>
       </c>
@@ -7343,7 +7149,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8">
+    <row r="8" spans="1:12" ht="30">
       <c r="A8" s="68">
         <v>45588</v>
       </c>
@@ -7363,7 +7169,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="A9" s="68">
         <v>45588</v>
       </c>
@@ -7383,7 +7189,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8">
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="68">
         <v>45588</v>
       </c>
@@ -7403,7 +7209,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18">
+    <row r="11" spans="1:12" ht="18.75">
       <c r="A11" s="68">
         <v>45589</v>
       </c>
@@ -7421,7 +7227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18">
+    <row r="12" spans="1:12" ht="18.75">
       <c r="A12" s="68">
         <v>45590</v>
       </c>
@@ -7441,7 +7247,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.8">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="68">
         <v>45593</v>
       </c>
@@ -7475,7 +7281,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42" style="86" bestFit="1" customWidth="1"/>
@@ -7490,7 +7296,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="14" t="s">
         <v>90</v>
       </c>
@@ -7501,7 +7307,7 @@
         <v>9599594524</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4">
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="14" t="s">
         <v>91</v>
       </c>
@@ -7512,8 +7318,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.4" thickBot="1"/>
-    <row r="10" spans="1:12" ht="91.2" thickTop="1" thickBot="1">
+    <row r="9" spans="1:12" ht="15" thickBot="1"/>
+    <row r="10" spans="1:12" ht="92.25" thickTop="1" thickBot="1">
       <c r="A10" s="84" t="s">
         <v>128</v>
       </c>
@@ -7551,7 +7357,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.4" thickTop="1"/>
+    <row r="11" spans="1:12" ht="15" thickTop="1"/>
     <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>95</v>
@@ -7611,7 +7417,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.4">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="12" t="s">
         <v>133</v>
       </c>
@@ -7653,7 +7459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.8">
+    <row r="26" spans="1:4" ht="23.25">
       <c r="A26" s="85" t="s">
         <v>93</v>
       </c>
@@ -7706,7 +7512,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="91" t="s">
@@ -7723,13 +7529,13 @@
   <dimension ref="A6:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>

</xml_diff>